<commit_message>
Updated program report page
- Include Max PE Silos as user defined
</commit_message>
<xml_diff>
--- a/Program Report Page.xlsx
+++ b/Program Report Page.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/Desktop/Codes + Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/Desktop/Scope 2/Codes + Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A5B2E16-C5B7-AE44-B835-0875D58BF921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD06E33D-5E93-8142-AD7F-F1D7203001E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="-7740" windowWidth="38400" windowHeight="21100" xr2:uid="{56F6261A-643D-D442-AAD7-D69978890D25}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Automated LTP Program</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t xml:space="preserve">Total Run Time </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max PE Silos Setting: </t>
   </si>
 </sst>
 </file>
@@ -205,13 +208,13 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -553,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A0674A6-7EE7-EC49-A7E5-3D8BB324C3CE}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -570,11 +573,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:9" ht="26" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -586,14 +589,14 @@
       <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="H2" s="7" t="s">
+      <c r="F2" s="8"/>
+      <c r="H2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="7"/>
+      <c r="I2" s="8"/>
     </row>
     <row r="3" spans="1:9" ht="24" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -631,7 +634,7 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="6" t="s">
         <v>15</v>
       </c>
       <c r="F5" s="1"/>
@@ -647,6 +650,12 @@
         <v>14</v>
       </c>
       <c r="B8" s="1"/>
+    </row>
+    <row r="10" spans="1:9" ht="24" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>